<commit_message>
Add Moz 2023 modified survey data, update some data cleaning for legacy data
</commit_message>
<xml_diff>
--- a/data-raw/hhs_questions.xlsx
+++ b/data-raw/hhs_questions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adu/Documents/rare/HHS_Dashboard/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{27A6E154-0AA6-FB43-A3A2-614FA467A5F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C6783B4-AAB0-7D4B-B00A-94DD70244DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="960" windowWidth="27240" windowHeight="15940" xr2:uid="{41E5930D-BBC6-7141-A308-84615B62A11C}"/>
+    <workbookView xWindow="1560" yWindow="960" windowWidth="27240" windowHeight="15940" xr2:uid="{41E5930D-BBC6-7141-A308-84615B62A11C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -5081,19 +5081,7 @@
     <t>61g</t>
   </si>
   <si>
-    <t>Please state your level of agreement with the following statement: g) Through my individual fishing behavior, I can make a meaningful contribution to the sustainability of the fish catch.</t>
-  </si>
-  <si>
     <t>Empowerment</t>
-  </si>
-  <si>
-    <t>Por favor, diga se você concorda ou discorda com as seguintes declarações: g) Através do meu comportamento individual, posso contribuir de forma significativa para a sustentabilidade da captura do pescado.</t>
-  </si>
-  <si>
-    <t>Por favor, indique o seu nível de concordância com a seguinte declaração: g) Através do meu comportamento individual de pesca, posso dar uma contribuição significativa para a sustentabilidade das capturas de peixe.</t>
-  </si>
-  <si>
-    <t>Sebutkan apakah Anda setuju dengan pernyataan berikut: g) Perilaku saya dalam hal menangkap ikan dapat memberikan kontribusi yang berarti bagi keberlanjutan hasil tangkapan.</t>
   </si>
   <si>
     <t xml:space="preserve">Indique su nivel de acuerdo con la siguiente afirmación:  f) A través de mi comportamiento individual como pescador puedo hacer una  contribución significativa a la sostenibilidad de las pesquerías
@@ -5106,22 +5094,10 @@
     <t>61h</t>
   </si>
   <si>
-    <t>Please state your level of agreement with the following statement: h) It is important for me to be able to help my neighbors in times of need</t>
-  </si>
-  <si>
     <t>Improve Well Being,
 Social Cohesion</t>
   </si>
   <si>
-    <t>Por favor, diga se você concorda ou discorda com as seguintes declarações: h) É importante para mim poder ajudar meus vizinhos em momentos de necessidade.</t>
-  </si>
-  <si>
-    <t>Por favor, indique o seu nível de concordância com a seguinte declaração: h) É importante para mim poder ajudar os meus vizinhos em momentos de necessidade.</t>
-  </si>
-  <si>
-    <t>Sebutkan apakah Anda setuju dengan pernyataan berikut: h) Penting bagi saya untuk dapat membantu tetangga saya pada saat dibutuhkan.</t>
-  </si>
-  <si>
     <t>Indique su nivel de acuerdo con la siguiente afirmación: g) En momento de necesidad, es importante para mí poder ayudar a mis vecinos</t>
   </si>
   <si>
@@ -5147,9 +5123,6 @@
   </si>
   <si>
     <t>61f</t>
-  </si>
-  <si>
-    <t>Please state your level of agreement with the following statement: h) I am willing to change my fishing behavior</t>
   </si>
   <si>
     <t>FFCR Indicator</t>
@@ -5985,6 +5958,33 @@
   </si>
   <si>
     <t>si, no, nombre de otro, numero de telefono de otro</t>
+  </si>
+  <si>
+    <t>Please state your level of agreement with the following statement: f) Through my individual fishing behavior, I can make a meaningful contribution to the sustainability of the fish catch.</t>
+  </si>
+  <si>
+    <t>Por favor, diga se você concorda ou discorda com as seguintes declarações: f) Através do meu comportamento individual, posso contribuir de forma significativa para a sustentabilidade da captura do pescado.</t>
+  </si>
+  <si>
+    <t>Por favor, indique o seu nível de concordância com a seguinte declaração: f) Através do meu comportamento individual de pesca, posso dar uma contribuição significativa para a sustentabilidade das capturas de peixe.</t>
+  </si>
+  <si>
+    <t>Sebutkan apakah Anda setuju dengan pernyataan berikut: f) Perilaku saya dalam hal menangkap ikan dapat memberikan kontribusi yang berarti bagi keberlanjutan hasil tangkapan.</t>
+  </si>
+  <si>
+    <t>Please state your level of agreement with the following statement: g) It is important for me to be able to help my neighbors in times of need</t>
+  </si>
+  <si>
+    <t>Por favor, diga se você concorda ou discorda com as seguintes declarações: g) É importante para mim poder ajudar meus vizinhos em momentos de necessidade.</t>
+  </si>
+  <si>
+    <t>Por favor, indique o seu nível de concordância com a seguinte declaração: g) É importante para mim poder ajudar os meus vizinhos em momentos de necessidade.</t>
+  </si>
+  <si>
+    <t>Sebutkan apakah Anda setuju dengan pernyataan berikut: g) Penting bagi saya untuk dapat membantu tetangga saya pada saat dibutuhkan.</t>
+  </si>
+  <si>
+    <t>Please state your level of agreement with the following statement: i) I am willing to change my fishing behavior</t>
   </si>
 </sst>
 </file>
@@ -6619,8 +6619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4953BA0E-E7CE-3548-B9BF-54B2EFB53F98}">
   <dimension ref="A1:T113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="I93" sqref="I93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11726,7 +11726,7 @@
         <v>91</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>1037</v>
+        <v>1245</v>
       </c>
       <c r="E90" s="5" t="s">
         <v>989</v>
@@ -11735,31 +11735,31 @@
         <v>118</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="H90" s="5" t="s">
         <v>23</v>
       </c>
       <c r="I90" s="6" t="s">
-        <v>1039</v>
+        <v>1246</v>
       </c>
       <c r="J90" s="7" t="s">
         <v>993</v>
       </c>
       <c r="K90" s="5" t="s">
-        <v>1040</v>
+        <v>1247</v>
       </c>
       <c r="L90" s="9" t="s">
         <v>995</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>1041</v>
+        <v>1248</v>
       </c>
       <c r="N90" s="7" t="s">
         <v>997</v>
       </c>
       <c r="O90" s="5" t="s">
-        <v>1042</v>
+        <v>1038</v>
       </c>
       <c r="P90" s="5" t="s">
         <v>936</v>
@@ -11771,16 +11771,16 @@
     </row>
     <row r="91" spans="1:20" ht="285" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>1043</v>
+        <v>1039</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>1044</v>
+        <v>1040</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>1045</v>
+        <v>1249</v>
       </c>
       <c r="E91" s="5" t="s">
         <v>989</v>
@@ -11789,31 +11789,31 @@
         <v>523</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>1046</v>
+        <v>1041</v>
       </c>
       <c r="H91" s="5" t="s">
         <v>525</v>
       </c>
       <c r="I91" s="6" t="s">
-        <v>1047</v>
+        <v>1250</v>
       </c>
       <c r="J91" s="7" t="s">
         <v>993</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>1048</v>
+        <v>1251</v>
       </c>
       <c r="L91" s="9" t="s">
         <v>995</v>
       </c>
       <c r="M91" s="7" t="s">
-        <v>1049</v>
+        <v>1252</v>
       </c>
       <c r="N91" s="7" t="s">
         <v>997</v>
       </c>
       <c r="O91" s="5" t="s">
-        <v>1050</v>
+        <v>1042</v>
       </c>
       <c r="P91" s="5" t="s">
         <v>936</v>
@@ -11825,7 +11825,7 @@
     </row>
     <row r="92" spans="1:20" ht="210" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>1051</v>
+        <v>1043</v>
       </c>
       <c r="B92" s="4" t="s">
         <v>130</v>
@@ -11834,7 +11834,7 @@
         <v>91</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>1052</v>
+        <v>1044</v>
       </c>
       <c r="E92" s="5" t="s">
         <v>989</v>
@@ -11849,25 +11849,25 @@
         <v>23</v>
       </c>
       <c r="I92" s="6" t="s">
-        <v>1053</v>
+        <v>1045</v>
       </c>
       <c r="J92" s="7" t="s">
         <v>993</v>
       </c>
       <c r="K92" s="5" t="s">
-        <v>1054</v>
+        <v>1046</v>
       </c>
       <c r="L92" s="9" t="s">
         <v>995</v>
       </c>
       <c r="M92" s="7" t="s">
-        <v>1055</v>
+        <v>1047</v>
       </c>
       <c r="N92" s="7" t="s">
         <v>997</v>
       </c>
       <c r="O92" s="5" t="s">
-        <v>1056</v>
+        <v>1048</v>
       </c>
       <c r="P92" s="5" t="s">
         <v>936</v>
@@ -11879,35 +11879,35 @@
     </row>
     <row r="93" spans="1:20" ht="208" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>1057</v>
+        <v>1049</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>1058</v>
+        <v>1050</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>1059</v>
+        <v>1253</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>989</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>1060</v>
+        <v>1051</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>1061</v>
+        <v>1052</v>
       </c>
       <c r="H93" s="5" t="s">
-        <v>1062</v>
+        <v>1053</v>
       </c>
       <c r="I93" s="6"/>
       <c r="J93" s="7"/>
       <c r="K93" s="5"/>
       <c r="L93" s="9"/>
       <c r="M93" s="7" t="s">
-        <v>1063</v>
+        <v>1054</v>
       </c>
       <c r="N93" s="7" t="s">
         <v>997</v>
@@ -11930,10 +11930,10 @@
         <v>91</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>1064</v>
+        <v>1055</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>1065</v>
+        <v>1056</v>
       </c>
       <c r="F94" s="5" t="s">
         <v>919</v>
@@ -11945,28 +11945,28 @@
         <v>23</v>
       </c>
       <c r="I94" s="6" t="s">
-        <v>1066</v>
+        <v>1057</v>
       </c>
       <c r="J94" s="7" t="s">
-        <v>1067</v>
+        <v>1058</v>
       </c>
       <c r="K94" s="5" t="s">
-        <v>1068</v>
+        <v>1059</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>1069</v>
+        <v>1060</v>
       </c>
       <c r="M94" s="7" t="s">
-        <v>1070</v>
+        <v>1061</v>
       </c>
       <c r="N94" s="7" t="s">
-        <v>1071</v>
+        <v>1062</v>
       </c>
       <c r="O94" s="5" t="s">
-        <v>1072</v>
+        <v>1063</v>
       </c>
       <c r="P94" s="5" t="s">
-        <v>1073</v>
+        <v>1064</v>
       </c>
       <c r="Q94" s="7"/>
       <c r="R94" s="7"/>
@@ -11984,43 +11984,43 @@
         <v>91</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>1074</v>
+        <v>1065</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>1075</v>
+        <v>1066</v>
       </c>
       <c r="F95" s="5" t="s">
         <v>251</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>1076</v>
+        <v>1067</v>
       </c>
       <c r="H95" s="5" t="s">
         <v>1022</v>
       </c>
       <c r="I95" s="6" t="s">
-        <v>1077</v>
+        <v>1068</v>
       </c>
       <c r="J95" s="7" t="s">
-        <v>1078</v>
+        <v>1069</v>
       </c>
       <c r="K95" s="5" t="s">
-        <v>1079</v>
+        <v>1070</v>
       </c>
       <c r="L95" s="9" t="s">
-        <v>1080</v>
+        <v>1071</v>
       </c>
       <c r="M95" s="7" t="s">
-        <v>1081</v>
+        <v>1072</v>
       </c>
       <c r="N95" s="7" t="s">
-        <v>1082</v>
+        <v>1073</v>
       </c>
       <c r="O95" s="5" t="s">
-        <v>1083</v>
+        <v>1074</v>
       </c>
       <c r="P95" s="5" t="s">
-        <v>1084</v>
+        <v>1075</v>
       </c>
       <c r="Q95" s="7"/>
       <c r="R95" s="7"/>
@@ -12032,16 +12032,16 @@
         <v>77</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>1085</v>
+        <v>1076</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>1086</v>
+        <v>1077</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>1087</v>
+        <v>1078</v>
       </c>
       <c r="F96" s="5" t="s">
         <v>251</v>
@@ -12053,28 +12053,28 @@
         <v>848</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>1088</v>
+        <v>1079</v>
       </c>
       <c r="J96" s="7" t="s">
-        <v>1089</v>
+        <v>1080</v>
       </c>
       <c r="K96" s="5" t="s">
-        <v>1090</v>
+        <v>1081</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>1091</v>
+        <v>1082</v>
       </c>
       <c r="M96" s="7" t="s">
-        <v>1092</v>
+        <v>1083</v>
       </c>
       <c r="N96" s="7" t="s">
-        <v>1093</v>
+        <v>1084</v>
       </c>
       <c r="O96" s="5" t="s">
-        <v>1094</v>
+        <v>1085</v>
       </c>
       <c r="P96" s="5" t="s">
-        <v>1095</v>
+        <v>1086</v>
       </c>
       <c r="Q96" s="7"/>
       <c r="R96" s="7"/>
@@ -12092,10 +12092,10 @@
         <v>91</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>1096</v>
+        <v>1087</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>1097</v>
+        <v>1088</v>
       </c>
       <c r="F97" s="5" t="s">
         <v>919</v>
@@ -12107,28 +12107,28 @@
         <v>23</v>
       </c>
       <c r="I97" s="6" t="s">
-        <v>1098</v>
+        <v>1089</v>
       </c>
       <c r="J97" s="7" t="s">
-        <v>1099</v>
+        <v>1090</v>
       </c>
       <c r="K97" s="5" t="s">
-        <v>1100</v>
+        <v>1091</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>1101</v>
+        <v>1092</v>
       </c>
       <c r="M97" s="7" t="s">
-        <v>1102</v>
+        <v>1093</v>
       </c>
       <c r="N97" s="7" t="s">
-        <v>1103</v>
+        <v>1094</v>
       </c>
       <c r="O97" s="5" t="s">
-        <v>1104</v>
+        <v>1095</v>
       </c>
       <c r="P97" s="5" t="s">
-        <v>1105</v>
+        <v>1096</v>
       </c>
       <c r="Q97" s="7"/>
       <c r="R97" s="7"/>
@@ -12146,10 +12146,10 @@
         <v>91</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>1106</v>
+        <v>1097</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>1107</v>
+        <v>1098</v>
       </c>
       <c r="F98" s="5" t="s">
         <v>919</v>
@@ -12161,28 +12161,28 @@
         <v>23</v>
       </c>
       <c r="I98" s="6" t="s">
-        <v>1108</v>
+        <v>1099</v>
       </c>
       <c r="J98" s="7" t="s">
-        <v>1109</v>
+        <v>1100</v>
       </c>
       <c r="K98" s="5" t="s">
-        <v>1110</v>
+        <v>1101</v>
       </c>
       <c r="L98" s="9" t="s">
-        <v>1111</v>
+        <v>1102</v>
       </c>
       <c r="M98" s="7" t="s">
-        <v>1112</v>
+        <v>1103</v>
       </c>
       <c r="N98" s="7" t="s">
-        <v>1113</v>
+        <v>1104</v>
       </c>
       <c r="O98" s="5" t="s">
-        <v>1114</v>
+        <v>1105</v>
       </c>
       <c r="P98" s="5" t="s">
-        <v>1115</v>
+        <v>1106</v>
       </c>
       <c r="Q98" s="7"/>
       <c r="R98" s="7"/>
@@ -12194,16 +12194,16 @@
         <v>80</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>1116</v>
+        <v>1107</v>
       </c>
       <c r="C99" s="4" t="s">
         <v>91</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>1117</v>
+        <v>1108</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>1118</v>
+        <v>1109</v>
       </c>
       <c r="F99" s="5" t="s">
         <v>919</v>
@@ -12215,28 +12215,28 @@
         <v>23</v>
       </c>
       <c r="I99" s="6" t="s">
-        <v>1119</v>
+        <v>1110</v>
       </c>
       <c r="J99" s="7" t="s">
-        <v>1120</v>
+        <v>1111</v>
       </c>
       <c r="K99" s="5" t="s">
-        <v>1121</v>
+        <v>1112</v>
       </c>
       <c r="L99" s="9" t="s">
-        <v>1120</v>
+        <v>1111</v>
       </c>
       <c r="M99" s="7" t="s">
-        <v>1122</v>
+        <v>1113</v>
       </c>
       <c r="N99" s="7" t="s">
-        <v>1123</v>
+        <v>1114</v>
       </c>
       <c r="O99" s="5" t="s">
-        <v>1124</v>
+        <v>1115</v>
       </c>
       <c r="P99" s="5" t="s">
-        <v>1125</v>
+        <v>1116</v>
       </c>
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
@@ -12251,13 +12251,13 @@
         <v>68</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>1126</v>
+        <v>1117</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>1127</v>
+        <v>1118</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>1128</v>
+        <v>1119</v>
       </c>
       <c r="F100" s="5" t="s">
         <v>171</v>
@@ -12266,31 +12266,31 @@
         <v>943</v>
       </c>
       <c r="H100" s="5" t="s">
-        <v>1129</v>
+        <v>1120</v>
       </c>
       <c r="I100" s="6" t="s">
-        <v>1130</v>
+        <v>1121</v>
       </c>
       <c r="J100" s="7" t="s">
-        <v>1131</v>
+        <v>1122</v>
       </c>
       <c r="K100" s="5" t="s">
-        <v>1132</v>
+        <v>1123</v>
       </c>
       <c r="L100" s="9" t="s">
-        <v>1133</v>
+        <v>1124</v>
       </c>
       <c r="M100" s="7" t="s">
-        <v>1134</v>
+        <v>1125</v>
       </c>
       <c r="N100" s="7" t="s">
-        <v>1135</v>
+        <v>1126</v>
       </c>
       <c r="O100" s="5" t="s">
-        <v>1136</v>
+        <v>1127</v>
       </c>
       <c r="P100" s="5" t="s">
-        <v>1131</v>
+        <v>1122</v>
       </c>
       <c r="Q100" s="7"/>
       <c r="R100" s="7"/>
@@ -12308,13 +12308,13 @@
         <v>91</v>
       </c>
       <c r="D101" s="29" t="s">
-        <v>1137</v>
+        <v>1128</v>
       </c>
       <c r="E101" s="29" t="s">
-        <v>1138</v>
+        <v>1129</v>
       </c>
       <c r="F101" s="29" t="s">
-        <v>1139</v>
+        <v>1130</v>
       </c>
       <c r="G101" s="29" t="s">
         <v>23</v>
@@ -12323,28 +12323,28 @@
         <v>23</v>
       </c>
       <c r="I101" s="37" t="s">
-        <v>1140</v>
+        <v>1131</v>
       </c>
       <c r="J101" s="30" t="s">
-        <v>1141</v>
+        <v>1132</v>
       </c>
       <c r="K101" s="29" t="s">
-        <v>1142</v>
+        <v>1133</v>
       </c>
       <c r="L101" s="32" t="s">
-        <v>1143</v>
+        <v>1134</v>
       </c>
       <c r="M101" s="30" t="s">
-        <v>1144</v>
+        <v>1135</v>
       </c>
       <c r="N101" s="30" t="s">
-        <v>1145</v>
+        <v>1136</v>
       </c>
       <c r="O101" s="29" t="s">
-        <v>1146</v>
+        <v>1137</v>
       </c>
       <c r="P101" s="29" t="s">
-        <v>1147</v>
+        <v>1138</v>
       </c>
       <c r="Q101" s="30"/>
       <c r="R101" s="30"/>
@@ -12362,10 +12362,10 @@
         <v>33</v>
       </c>
       <c r="D102" s="5" t="s">
-        <v>1148</v>
+        <v>1139</v>
       </c>
       <c r="E102" s="5" t="s">
-        <v>1149</v>
+        <v>1140</v>
       </c>
       <c r="F102" s="5" t="s">
         <v>171</v>
@@ -12374,31 +12374,31 @@
         <v>172</v>
       </c>
       <c r="H102" s="5" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="I102" s="6" t="s">
-        <v>1151</v>
+        <v>1142</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>1152</v>
+        <v>1143</v>
       </c>
       <c r="K102" s="5" t="s">
-        <v>1153</v>
+        <v>1144</v>
       </c>
       <c r="L102" s="9" t="s">
-        <v>1154</v>
+        <v>1145</v>
       </c>
       <c r="M102" s="7" t="s">
-        <v>1155</v>
+        <v>1146</v>
       </c>
       <c r="N102" s="7" t="s">
-        <v>1156</v>
+        <v>1147</v>
       </c>
       <c r="O102" s="5" t="s">
-        <v>1157</v>
+        <v>1148</v>
       </c>
       <c r="P102" s="5" t="s">
-        <v>1158</v>
+        <v>1149</v>
       </c>
       <c r="Q102" s="7"/>
       <c r="R102" s="7"/>
@@ -12413,13 +12413,13 @@
         <v>71</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>1159</v>
+        <v>1150</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>1160</v>
+        <v>1151</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>1161</v>
+        <v>1152</v>
       </c>
       <c r="F103" s="5" t="s">
         <v>171</v>
@@ -12431,28 +12431,28 @@
         <v>173</v>
       </c>
       <c r="I103" s="6" t="s">
-        <v>1162</v>
+        <v>1153</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>1163</v>
+        <v>1154</v>
       </c>
       <c r="K103" s="5" t="s">
-        <v>1164</v>
+        <v>1155</v>
       </c>
       <c r="L103" s="9" t="s">
-        <v>1165</v>
+        <v>1156</v>
       </c>
       <c r="M103" s="7" t="s">
-        <v>1166</v>
+        <v>1157</v>
       </c>
       <c r="N103" s="7" t="s">
-        <v>1167</v>
+        <v>1158</v>
       </c>
       <c r="O103" s="5" t="s">
-        <v>1168</v>
+        <v>1159</v>
       </c>
       <c r="P103" s="5" t="s">
-        <v>1169</v>
+        <v>1160</v>
       </c>
       <c r="Q103" s="7"/>
       <c r="R103" s="7"/>
@@ -12470,10 +12470,10 @@
         <v>601</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>1170</v>
+        <v>1161</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>1171</v>
+        <v>1162</v>
       </c>
       <c r="F104" s="5" t="s">
         <v>171</v>
@@ -12482,31 +12482,31 @@
         <v>172</v>
       </c>
       <c r="H104" s="5" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="I104" s="6" t="s">
-        <v>1173</v>
+        <v>1164</v>
       </c>
       <c r="J104" s="7" t="s">
-        <v>1174</v>
+        <v>1165</v>
       </c>
       <c r="K104" s="5" t="s">
-        <v>1175</v>
+        <v>1166</v>
       </c>
       <c r="L104" s="9" t="s">
-        <v>1176</v>
+        <v>1167</v>
       </c>
       <c r="M104" s="7" t="s">
-        <v>1177</v>
+        <v>1168</v>
       </c>
       <c r="N104" s="7" t="s">
-        <v>1178</v>
+        <v>1169</v>
       </c>
       <c r="O104" s="5" t="s">
-        <v>1179</v>
+        <v>1170</v>
       </c>
       <c r="P104" s="5" t="s">
-        <v>1180</v>
+        <v>1171</v>
       </c>
       <c r="Q104" s="7"/>
       <c r="R104" s="7"/>
@@ -12524,10 +12524,10 @@
         <v>91</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>1181</v>
+        <v>1172</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>1171</v>
+        <v>1162</v>
       </c>
       <c r="F105" s="5" t="s">
         <v>171</v>
@@ -12536,31 +12536,31 @@
         <v>172</v>
       </c>
       <c r="H105" s="5" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="I105" s="6" t="s">
-        <v>1182</v>
+        <v>1173</v>
       </c>
       <c r="J105" s="7" t="s">
+        <v>1165</v>
+      </c>
+      <c r="K105" s="5" t="s">
         <v>1174</v>
       </c>
-      <c r="K105" s="5" t="s">
-        <v>1183</v>
-      </c>
       <c r="L105" s="9" t="s">
+        <v>1167</v>
+      </c>
+      <c r="M105" s="7" t="s">
+        <v>1175</v>
+      </c>
+      <c r="N105" s="7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="O105" s="5" t="s">
         <v>1176</v>
       </c>
-      <c r="M105" s="7" t="s">
-        <v>1184</v>
-      </c>
-      <c r="N105" s="7" t="s">
-        <v>1178</v>
-      </c>
-      <c r="O105" s="5" t="s">
-        <v>1185</v>
-      </c>
       <c r="P105" s="5" t="s">
-        <v>1180</v>
+        <v>1171</v>
       </c>
       <c r="Q105" s="7"/>
       <c r="R105" s="7"/>
@@ -12578,10 +12578,10 @@
         <v>91</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>1186</v>
+        <v>1177</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="F106" s="5" t="s">
         <v>171</v>
@@ -12590,31 +12590,31 @@
         <v>172</v>
       </c>
       <c r="H106" s="5" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="I106" s="6" t="s">
-        <v>1188</v>
+        <v>1179</v>
       </c>
       <c r="J106" s="7" t="s">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="K106" s="5" t="s">
-        <v>1190</v>
+        <v>1181</v>
       </c>
       <c r="L106" s="9" t="s">
-        <v>1191</v>
+        <v>1182</v>
       </c>
       <c r="M106" s="7" t="s">
-        <v>1192</v>
+        <v>1183</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="O106" s="5" t="s">
-        <v>1194</v>
+        <v>1185</v>
       </c>
       <c r="P106" s="5" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
       <c r="Q106" s="7"/>
       <c r="R106" s="7"/>
@@ -12632,10 +12632,10 @@
         <v>91</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>1196</v>
+        <v>1187</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="F107" s="5" t="s">
         <v>171</v>
@@ -12644,31 +12644,31 @@
         <v>172</v>
       </c>
       <c r="H107" s="5" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>1197</v>
+        <v>1188</v>
       </c>
       <c r="J107" s="7" t="s">
+        <v>1180</v>
+      </c>
+      <c r="K107" s="5" t="s">
         <v>1189</v>
       </c>
-      <c r="K107" s="5" t="s">
-        <v>1198</v>
-      </c>
       <c r="L107" s="9" t="s">
+        <v>1182</v>
+      </c>
+      <c r="M107" s="7" t="s">
+        <v>1190</v>
+      </c>
+      <c r="N107" s="7" t="s">
+        <v>1184</v>
+      </c>
+      <c r="O107" s="5" t="s">
         <v>1191</v>
       </c>
-      <c r="M107" s="7" t="s">
-        <v>1199</v>
-      </c>
-      <c r="N107" s="7" t="s">
-        <v>1193</v>
-      </c>
-      <c r="O107" s="5" t="s">
-        <v>1200</v>
-      </c>
       <c r="P107" s="5" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
       <c r="Q107" s="7"/>
       <c r="R107" s="7"/>
@@ -12686,10 +12686,10 @@
         <v>91</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>1201</v>
+        <v>1192</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>1187</v>
+        <v>1178</v>
       </c>
       <c r="F108" s="5" t="s">
         <v>171</v>
@@ -12698,31 +12698,31 @@
         <v>172</v>
       </c>
       <c r="H108" s="5" t="s">
-        <v>1150</v>
+        <v>1141</v>
       </c>
       <c r="I108" s="6" t="s">
-        <v>1202</v>
+        <v>1193</v>
       </c>
       <c r="J108" s="7" t="s">
-        <v>1189</v>
+        <v>1180</v>
       </c>
       <c r="K108" s="5" t="s">
-        <v>1203</v>
+        <v>1194</v>
       </c>
       <c r="L108" s="9" t="s">
-        <v>1191</v>
+        <v>1182</v>
       </c>
       <c r="M108" s="7" t="s">
-        <v>1204</v>
+        <v>1195</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>1193</v>
+        <v>1184</v>
       </c>
       <c r="O108" s="5" t="s">
-        <v>1205</v>
+        <v>1196</v>
       </c>
       <c r="P108" s="5" t="s">
-        <v>1195</v>
+        <v>1186</v>
       </c>
       <c r="Q108" s="7"/>
       <c r="R108" s="7"/>
@@ -12734,16 +12734,16 @@
         <v>90</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>1206</v>
+        <v>1197</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>1207</v>
+        <v>1198</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>1208</v>
+        <v>1199</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>1209</v>
+        <v>1200</v>
       </c>
       <c r="F109" s="5" t="s">
         <v>171</v>
@@ -12752,31 +12752,31 @@
         <v>172</v>
       </c>
       <c r="H109" s="5" t="s">
-        <v>1172</v>
+        <v>1163</v>
       </c>
       <c r="I109" s="6" t="s">
-        <v>1210</v>
+        <v>1201</v>
       </c>
       <c r="J109" s="7" t="s">
-        <v>1211</v>
+        <v>1202</v>
       </c>
       <c r="K109" s="5" t="s">
-        <v>1212</v>
+        <v>1203</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>1213</v>
+        <v>1204</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>1214</v>
+        <v>1205</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>1215</v>
+        <v>1206</v>
       </c>
       <c r="O109" s="5" t="s">
-        <v>1216</v>
+        <v>1207</v>
       </c>
       <c r="P109" s="5" t="s">
-        <v>1217</v>
+        <v>1208</v>
       </c>
       <c r="Q109" s="7"/>
       <c r="R109" s="7"/>
@@ -12788,16 +12788,16 @@
         <v>91</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>1218</v>
+        <v>1209</v>
       </c>
       <c r="C110" s="4">
         <v>37</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>1219</v>
+        <v>1210</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>1220</v>
+        <v>1211</v>
       </c>
       <c r="F110" s="5" t="s">
         <v>251</v>
@@ -12806,31 +12806,31 @@
         <v>724</v>
       </c>
       <c r="H110" s="5" t="s">
-        <v>1221</v>
+        <v>1212</v>
       </c>
       <c r="I110" s="6" t="s">
-        <v>1222</v>
+        <v>1213</v>
       </c>
       <c r="J110" s="7" t="s">
-        <v>1223</v>
+        <v>1214</v>
       </c>
       <c r="K110" s="5" t="s">
-        <v>1224</v>
+        <v>1215</v>
       </c>
       <c r="L110" s="9" t="s">
-        <v>1225</v>
+        <v>1216</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>1226</v>
+        <v>1217</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>1227</v>
+        <v>1218</v>
       </c>
       <c r="O110" s="5" t="s">
-        <v>1228</v>
+        <v>1219</v>
       </c>
       <c r="P110" s="5" t="s">
-        <v>1229</v>
+        <v>1220</v>
       </c>
       <c r="Q110" s="7"/>
       <c r="R110" s="7"/>
@@ -12848,7 +12848,7 @@
         <v>43</v>
       </c>
       <c r="D111" s="29" t="s">
-        <v>1230</v>
+        <v>1221</v>
       </c>
       <c r="E111" s="29" t="s">
         <v>300</v>
@@ -12863,25 +12863,25 @@
         <v>23</v>
       </c>
       <c r="I111" s="37" t="s">
-        <v>1231</v>
+        <v>1222</v>
       </c>
       <c r="J111" s="30" t="s">
         <v>304</v>
       </c>
       <c r="K111" s="29" t="s">
-        <v>1232</v>
+        <v>1223</v>
       </c>
       <c r="L111" s="32" t="s">
         <v>304</v>
       </c>
       <c r="M111" s="30" t="s">
-        <v>1233</v>
+        <v>1224</v>
       </c>
       <c r="N111" s="30" t="s">
         <v>308</v>
       </c>
       <c r="O111" s="29" t="s">
-        <v>1234</v>
+        <v>1225</v>
       </c>
       <c r="P111" s="29" t="s">
         <v>310</v>
@@ -12902,10 +12902,10 @@
         <v>44</v>
       </c>
       <c r="D112" s="29" t="s">
-        <v>1235</v>
+        <v>1226</v>
       </c>
       <c r="E112" s="29" t="s">
-        <v>1236</v>
+        <v>1227</v>
       </c>
       <c r="F112" s="29" t="s">
         <v>22</v>
@@ -12917,25 +12917,25 @@
         <v>23</v>
       </c>
       <c r="I112" s="37" t="s">
-        <v>1237</v>
+        <v>1228</v>
       </c>
       <c r="J112" s="30" t="s">
-        <v>1238</v>
+        <v>1229</v>
       </c>
       <c r="K112" s="29" t="s">
-        <v>1239</v>
+        <v>1230</v>
       </c>
       <c r="L112" s="32" t="s">
-        <v>1240</v>
+        <v>1231</v>
       </c>
       <c r="M112" s="30" t="s">
-        <v>1241</v>
+        <v>1232</v>
       </c>
       <c r="N112" s="30" t="s">
         <v>28</v>
       </c>
       <c r="O112" s="29" t="s">
-        <v>1242</v>
+        <v>1233</v>
       </c>
       <c r="P112" s="29" t="s">
         <v>30</v>
@@ -12953,13 +12953,13 @@
         <v>81</v>
       </c>
       <c r="C113" s="43" t="s">
-        <v>1243</v>
+        <v>1234</v>
       </c>
       <c r="D113" s="45" t="s">
-        <v>1244</v>
+        <v>1235</v>
       </c>
       <c r="E113" s="45" t="s">
-        <v>1245</v>
+        <v>1236</v>
       </c>
       <c r="F113" s="45" t="s">
         <v>22</v>
@@ -12971,28 +12971,28 @@
         <v>23</v>
       </c>
       <c r="I113" s="37" t="s">
-        <v>1246</v>
+        <v>1237</v>
       </c>
       <c r="J113" s="30" t="s">
-        <v>1247</v>
+        <v>1238</v>
       </c>
       <c r="K113" s="29" t="s">
-        <v>1248</v>
+        <v>1239</v>
       </c>
       <c r="L113" s="32" t="s">
-        <v>1249</v>
+        <v>1240</v>
       </c>
       <c r="M113" s="30" t="s">
-        <v>1250</v>
+        <v>1241</v>
       </c>
       <c r="N113" s="30" t="s">
-        <v>1251</v>
+        <v>1242</v>
       </c>
       <c r="O113" s="45" t="s">
-        <v>1252</v>
+        <v>1243</v>
       </c>
       <c r="P113" s="45" t="s">
-        <v>1253</v>
+        <v>1244</v>
       </c>
       <c r="Q113" s="30"/>
       <c r="R113" s="30"/>

</xml_diff>